<commit_message>
Added regex for admin code.
</commit_message>
<xml_diff>
--- a/db/PCVH_FCVH.xlsx
+++ b/db/PCVH_FCVH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59B8F488-FE9B-4D0F-9C41-EF8717C2094C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79072B47-BCD1-4610-A735-60C35B9731B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47532" yWindow="8304" windowWidth="21588" windowHeight="11136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="133">
   <si>
     <t>Case</t>
   </si>
@@ -401,6 +401,24 @@
   </si>
   <si>
     <t>4511.13C</t>
+  </si>
+  <si>
+    <t>22TRC00570</t>
+  </si>
+  <si>
+    <t>22TRC00570-A</t>
+  </si>
+  <si>
+    <t>Kudela</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>1501.17-5-04</t>
   </si>
 </sst>
 </file>
@@ -876,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1925,7 +1943,38 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="23.55" customHeight="1"/>
+    <row r="30" spans="1:12" ht="23.55" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added admin code two mid digits.
</commit_message>
<xml_diff>
--- a/db/PCVH_FCVH.xlsx
+++ b/db/PCVH_FCVH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79072B47-BCD1-4610-A735-60C35B9731B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCDE48A-CA3F-4D5D-8F4F-29613CB96811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47532" yWindow="8304" windowWidth="21588" windowHeight="11136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="139">
   <si>
     <t>Case</t>
   </si>
@@ -419,6 +419,24 @@
   </si>
   <si>
     <t>1501.17-5-04</t>
+  </si>
+  <si>
+    <t>22TRC00571</t>
+  </si>
+  <si>
+    <t>22TRC00571-A</t>
+  </si>
+  <si>
+    <t>Mick</t>
+  </si>
+  <si>
+    <t>Jagger</t>
+  </si>
+  <si>
+    <t>Test TWO</t>
+  </si>
+  <si>
+    <t>1501.17-11-01</t>
   </si>
 </sst>
 </file>
@@ -892,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1975,6 +1993,37 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
     </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>